<commit_message>
Check surround cells are not affected by merging cells
</commit_message>
<xml_diff>
--- a/test/files/merged_ranges.xlsx
+++ b/test/files/merged_ranges.xlsx
@@ -42,7 +42,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -58,6 +58,20 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,10 +91,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -88,22 +114,38 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,7 +500,7 @@
   <dimension ref="A1:IV19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -481,83 +523,93 @@
       <c r="IU2"/>
       <c r="IV2"/>
     </row>
-    <row r="3" spans="1:256" s="5" customFormat="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="IU3"/>
-      <c r="IV3"/>
+    <row r="3" spans="1:256" s="14" customFormat="1">
+      <c r="A3" s="13"/>
     </row>
     <row r="4" spans="1:256">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:256">
-      <c r="A5" s="10"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:256">
-      <c r="A6" s="10"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:256">
-      <c r="A7" s="9"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:256">
+      <c r="A8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:256">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:256">
-      <c r="A8" s="9"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:256">
-      <c r="A9" s="9"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:256">
-      <c r="A10" s="9"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="12"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:256">
-      <c r="A11" s="9"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="12"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:256">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="12"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:256">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="19" spans="2:2">
@@ -565,13 +617,14 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B7:D10"/>
-    <mergeCell ref="E4:E10"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:G10"/>
     <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B9:D12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>